<commit_message>
Sprint 3 - updated self assessment
</commit_message>
<xml_diff>
--- a/PI-2024-25_Team-Self-Assessment_SPRINT_3_v05.xlsx
+++ b/PI-2024-25_Team-Self-Assessment_SPRINT_3_v05.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonca\IdeaProjects\sem2-pi-24.25-g112-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC79F7C-5799-4EF1-ACB1-1A27AAC23499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F364FF9-06A0-4A0F-AF7D-4DD3A3068DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,15 +35,12 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="PAl2ezrMNVgdaSLMs7gw0/SIqw19XufJmCQ4PIcIU7E="/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="61">
   <si>
     <t>LAPR2 Project: Group/Team and Self-assessment v5.0</t>
   </si>
@@ -235,13 +232,16 @@
   </si>
   <si>
     <t>US25</t>
+  </si>
+  <si>
+    <t>User Manual (LAPR2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,6 +285,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -318,7 +325,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -888,11 +895,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1043,9 +1066,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{3DDE326F-86F8-4994-B1E8-3C82A10B8155}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1939,7 +1966,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2653,9 +2680,15 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="42"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
+      <c r="A27" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="48">
+        <v>1221919</v>
+      </c>
+      <c r="C27" s="48">
+        <v>5</v>
+      </c>
       <c r="D27" s="49"/>
       <c r="E27" s="42" t="s">
         <v>33</v>

</xml_diff>